<commit_message>
Doc: actualizacion del contenedor sia 55 a su ultima version
</commit_message>
<xml_diff>
--- a/modulo_odoo/Informes/Informexls/Inf_His_ComprasA.xlsx
+++ b/modulo_odoo/Informes/Informexls/Inf_His_ComprasA.xlsx
@@ -16,9 +16,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
-  <si>
-    <t>Informe Reclamacion Por Cliente a Corte: 09 - diciembre - 2021</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
+  <si>
+    <t>Informe Reclamacion Por Cliente a Corte: 10 - junio - 2022</t>
   </si>
   <si>
     <t>No.</t>
@@ -51,61 +51,67 @@
     <t>Estado Orden</t>
   </si>
   <si>
-    <t>FEPO1002001880</t>
-  </si>
-  <si>
-    <t>SO1755</t>
-  </si>
-  <si>
-    <t>Z7-Salida Reclamación Promocional/Ofertas Portos</t>
-  </si>
-  <si>
-    <t>BODEGA-008-CEDI PORTOS</t>
-  </si>
-  <si>
-    <t>VIR000070</t>
-  </si>
-  <si>
-    <t>ENDOGARD 2.5 2 TABLETAS</t>
-  </si>
-  <si>
-    <t>DROGUERIA Y VETERINARIA LTDA.</t>
-  </si>
-  <si>
-    <t>2021-02-27 16:03:05</t>
-  </si>
-  <si>
-    <t>done</t>
-  </si>
-  <si>
-    <t>SO1804</t>
-  </si>
-  <si>
-    <t>2021-03-05 15:08:57</t>
-  </si>
-  <si>
-    <t>SO1756</t>
-  </si>
-  <si>
-    <t>2021-02-27 18:10:17</t>
+    <t>77 - SALIDA ARECLAMACION OFERTA NR -005</t>
+  </si>
+  <si>
+    <t>SO5177</t>
+  </si>
+  <si>
+    <t>Z7 - SALIDA RECLAMACION PROMOCIONAL/ OFERTAS PORTOS 008</t>
+  </si>
+  <si>
+    <t>BODEGA-040-DIGITAL</t>
+  </si>
+  <si>
+    <t>CAMILA DELGADO</t>
+  </si>
+  <si>
+    <t>2022-03-29 13:59:23</t>
   </si>
   <si>
     <t>cancel</t>
   </si>
   <si>
-    <t>SO1803</t>
-  </si>
-  <si>
-    <t>2021-03-05 14:56:14</t>
-  </si>
-  <si>
-    <t>progress</t>
-  </si>
-  <si>
-    <t>SO1802</t>
-  </si>
-  <si>
-    <t>2021-03-05 14:50:39</t>
+    <t>SO4965</t>
+  </si>
+  <si>
+    <t>DUITAMA MARIA DE JESUS</t>
+  </si>
+  <si>
+    <t>2022-03-25 17:16:29</t>
+  </si>
+  <si>
+    <t>SO5383</t>
+  </si>
+  <si>
+    <t>RICHARD ALEJANDRO ALVAREZ</t>
+  </si>
+  <si>
+    <t>2022-04-08 16:07:40</t>
+  </si>
+  <si>
+    <t>SO5581</t>
+  </si>
+  <si>
+    <t>MACIAS TAMAYO HECTOR ARIEL</t>
+  </si>
+  <si>
+    <t>2022-04-21 13:54:03</t>
+  </si>
+  <si>
+    <t>SO5861</t>
+  </si>
+  <si>
+    <t>JAIR GARCIA</t>
+  </si>
+  <si>
+    <t>2022-04-25 21:42:16</t>
+  </si>
+  <si>
+    <t>SO5341</t>
+  </si>
+  <si>
+    <t>2022-03-30 15:20:59</t>
   </si>
 </sst>
 </file>
@@ -459,7 +465,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="C1" sqref="C1"/>
@@ -520,33 +526,17 @@
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3"/>
+      <c r="C3"/>
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" t="s">
-        <v>19</v>
-      </c>
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="H3"/>
+      <c r="I3"/>
+      <c r="J3"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4">
@@ -554,7 +544,7 @@
       </c>
       <c r="B4"/>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
@@ -565,13 +555,13 @@
       <c r="F4"/>
       <c r="G4"/>
       <c r="H4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" t="s">
         <v>17</v>
-      </c>
-      <c r="I4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J4" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -580,7 +570,7 @@
       </c>
       <c r="B5"/>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
@@ -591,13 +581,13 @@
       <c r="F5"/>
       <c r="G5"/>
       <c r="H5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" t="s">
         <v>17</v>
-      </c>
-      <c r="I5" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -606,7 +596,7 @@
       </c>
       <c r="B6"/>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
         <v>13</v>
@@ -617,13 +607,13 @@
       <c r="F6"/>
       <c r="G6"/>
       <c r="H6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" t="s">
         <v>17</v>
-      </c>
-      <c r="I6" t="s">
-        <v>26</v>
-      </c>
-      <c r="J6" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -632,7 +622,7 @@
       </c>
       <c r="B7"/>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
@@ -643,38 +633,66 @@
       <c r="F7"/>
       <c r="G7"/>
       <c r="H7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" t="s">
         <v>17</v>
       </c>
-      <c r="I7" t="s">
-        <v>29</v>
-      </c>
-      <c r="J7" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8"/>
+      <c r="A8">
+        <v>6</v>
+      </c>
       <c r="B8"/>
-      <c r="C8"/>
-      <c r="D8"/>
-      <c r="E8"/>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
       <c r="F8"/>
       <c r="G8"/>
-      <c r="H8"/>
-      <c r="I8"/>
-      <c r="J8"/>
+      <c r="H8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9"/>
+      <c r="A9">
+        <v>7</v>
+      </c>
       <c r="B9"/>
-      <c r="C9"/>
-      <c r="D9"/>
-      <c r="E9"/>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
       <c r="F9"/>
       <c r="G9"/>
-      <c r="H9"/>
-      <c r="I9"/>
-      <c r="J9"/>
+      <c r="H9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" t="s">
+        <v>31</v>
+      </c>
+      <c r="J9" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10"/>
@@ -747,6 +765,90 @@
       <c r="H15"/>
       <c r="I15"/>
       <c r="J15"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16"/>
+      <c r="B16"/>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
+      <c r="F16"/>
+      <c r="G16"/>
+      <c r="H16"/>
+      <c r="I16"/>
+      <c r="J16"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17"/>
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="F17"/>
+      <c r="G17"/>
+      <c r="H17"/>
+      <c r="I17"/>
+      <c r="J17"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18"/>
+      <c r="B18"/>
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="E18"/>
+      <c r="F18"/>
+      <c r="G18"/>
+      <c r="H18"/>
+      <c r="I18"/>
+      <c r="J18"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19"/>
+      <c r="B19"/>
+      <c r="C19"/>
+      <c r="D19"/>
+      <c r="E19"/>
+      <c r="F19"/>
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="I19"/>
+      <c r="J19"/>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20"/>
+      <c r="B20"/>
+      <c r="C20"/>
+      <c r="D20"/>
+      <c r="E20"/>
+      <c r="F20"/>
+      <c r="G20"/>
+      <c r="H20"/>
+      <c r="I20"/>
+      <c r="J20"/>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21"/>
+      <c r="B21"/>
+      <c r="C21"/>
+      <c r="D21"/>
+      <c r="E21"/>
+      <c r="F21"/>
+      <c r="G21"/>
+      <c r="H21"/>
+      <c r="I21"/>
+      <c r="J21"/>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22"/>
+      <c r="B22"/>
+      <c r="C22"/>
+      <c r="D22"/>
+      <c r="E22"/>
+      <c r="F22"/>
+      <c r="G22"/>
+      <c r="H22"/>
+      <c r="I22"/>
+      <c r="J22"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>